<commit_message>
Wrote more code for studets.
</commit_message>
<xml_diff>
--- a/PS_Search_Algorithms/path_planning_test.xlsx
+++ b/PS_Search_Algorithms/path_planning_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="space" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -44,8 +44,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -53,13 +59,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,173 +363,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -515,10 +555,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,46 +567,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>0.75</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>0.75</v>
       </c>
-      <c r="C2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="B3">
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B4">
         <v>0.25</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="1">
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0.5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C5">
         <v>1</v>
       </c>
     </row>
@@ -578,45 +623,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>0.5</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="B2">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="B3">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="C3">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -624,9 +658,20 @@
         <v>0.5</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.5</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="C5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added feature, that studetns will have access to 3 example human trajectories through Git
</commit_message>
<xml_diff>
--- a/PS_Search_Algorithms/path_planning_test.xlsx
+++ b/PS_Search_Algorithms/path_planning_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="space" sheetId="1" r:id="rId1"/>
@@ -78,11 +78,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,8 +366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,7 +397,7 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="4">
         <v>1</v>
       </c>
       <c r="G2" s="2"/>
@@ -444,7 +445,7 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
       <c r="B5" s="2">
@@ -625,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated somethings, when sitting with Roma
</commit_message>
<xml_diff>
--- a/PS_Search_Algorithms/path_planning_test.xlsx
+++ b/PS_Search_Algorithms/path_planning_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="space" sheetId="1" r:id="rId1"/>
@@ -366,8 +366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -386,7 +386,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -626,15 +626,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="B2">
         <v>1</v>

</xml_diff>